<commit_message>
Exact K-Means optimizer works
</commit_message>
<xml_diff>
--- a/src/a.xlsx
+++ b/src/a.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cygwin64\home\heins\GitHub\Trains\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\cygwin64\home\s.hein\GitHub\Trains\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{735596BE-6DD8-43A1-B4F2-38833CF488E0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="14220"/>
+    <workbookView xWindow="2415" yWindow="0" windowWidth="27870" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>sec</t>
   </si>
@@ -32,13 +33,25 @@
   <si>
     <t>m</t>
   </si>
+  <si>
+    <t>wheels</t>
+  </si>
+  <si>
+    <t>intra</t>
+  </si>
+  <si>
+    <t>inter</t>
+  </si>
+  <si>
+    <t>inter (wrong)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -519,7 +532,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -579,7 +592,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -593,7 +606,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -667,166 +679,166 @@
                   <c:v>10804</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>11819</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>12179</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>12539</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>13121</c:v>
+                  <c:v>12761</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13421</c:v>
+                  <c:v>13061</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15701</c:v>
+                  <c:v>15041</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16001</c:v>
+                  <c:v>15341</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16589</c:v>
+                  <c:v>15929</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16889</c:v>
+                  <c:v>16229</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19169</c:v>
+                  <c:v>18209</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19469</c:v>
+                  <c:v>18509</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20057</c:v>
+                  <c:v>19097</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20357</c:v>
+                  <c:v>19397</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22637</c:v>
+                  <c:v>21377</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22937</c:v>
+                  <c:v>21677</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23525</c:v>
+                  <c:v>22265</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>23825</c:v>
+                  <c:v>22565</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26105</c:v>
+                  <c:v>24545</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>26405</c:v>
+                  <c:v>24845</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>26993</c:v>
+                  <c:v>25433</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>27293</c:v>
+                  <c:v>25733</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>29573</c:v>
+                  <c:v>27713</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>29873</c:v>
+                  <c:v>28013</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>30461</c:v>
+                  <c:v>28601</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>30761</c:v>
+                  <c:v>28901</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>33041</c:v>
+                  <c:v>30881</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>33341</c:v>
+                  <c:v>31181</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>33929</c:v>
+                  <c:v>31769</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>34229</c:v>
+                  <c:v>32069</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>36509</c:v>
+                  <c:v>34049</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>36809</c:v>
+                  <c:v>34349</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>37397</c:v>
+                  <c:v>34937</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>37697</c:v>
+                  <c:v>35237</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>39977</c:v>
+                  <c:v>37217</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>40277</c:v>
+                  <c:v>37517</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>40865</c:v>
+                  <c:v>38105</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>41165</c:v>
+                  <c:v>38405</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>43445</c:v>
+                  <c:v>40385</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>43745</c:v>
+                  <c:v>40685</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>44333</c:v>
+                  <c:v>41273</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>44633</c:v>
+                  <c:v>41573</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>46913</c:v>
+                  <c:v>43553</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>47213</c:v>
+                  <c:v>43853</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>47801</c:v>
+                  <c:v>44441</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>48101</c:v>
+                  <c:v>44741</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>50381</c:v>
+                  <c:v>46721</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>50681</c:v>
+                  <c:v>47021</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>51269</c:v>
+                  <c:v>47609</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>51569</c:v>
+                  <c:v>47909</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>53849</c:v>
+                  <c:v>49889</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>54149</c:v>
+                  <c:v>50189</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>54887</c:v>
+                  <c:v>50927</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>55247</c:v>
+                  <c:v>51287</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>56622</c:v>
+                  <c:v>52302</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>56982</c:v>
+                  <c:v>52662</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1009,6 +1021,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A907-40AE-BAC3-405DCE915EF9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1042,145 +1059,145 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="47"/>
                 <c:pt idx="0">
-                  <c:v>12537</c:v>
+                  <c:v>10806</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13573</c:v>
+                  <c:v>11809</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15697</c:v>
+                  <c:v>12217</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16025</c:v>
+                  <c:v>12754</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16587</c:v>
+                  <c:v>13074</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16902</c:v>
+                  <c:v>15021</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19147</c:v>
+                  <c:v>15339</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19474</c:v>
+                  <c:v>15944</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20085</c:v>
+                  <c:v>16186</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20341</c:v>
+                  <c:v>18203</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22636</c:v>
+                  <c:v>18512</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22937</c:v>
+                  <c:v>19101</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23505</c:v>
+                  <c:v>19393</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23856</c:v>
+                  <c:v>21367</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>26105</c:v>
+                  <c:v>21676</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26404</c:v>
+                  <c:v>22254</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>26956</c:v>
+                  <c:v>22487</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>27241</c:v>
+                  <c:v>24582</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>29548</c:v>
+                  <c:v>24913</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>29924</c:v>
+                  <c:v>25444</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>30455</c:v>
+                  <c:v>25709</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>30770</c:v>
+                  <c:v>27707</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>33067</c:v>
+                  <c:v>28015</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>33304</c:v>
+                  <c:v>28585</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>33937</c:v>
+                  <c:v>28729</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>34238</c:v>
+                  <c:v>30883</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>36521</c:v>
+                  <c:v>31147</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>36746</c:v>
+                  <c:v>31784</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>37410</c:v>
+                  <c:v>32359</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>37704</c:v>
+                  <c:v>34041</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>39965</c:v>
+                  <c:v>34317</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>40309</c:v>
+                  <c:v>34933</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>40882</c:v>
+                  <c:v>35224</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>41242</c:v>
+                  <c:v>37206</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>43437</c:v>
+                  <c:v>37578</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>43727</c:v>
+                  <c:v>38106</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>44357</c:v>
+                  <c:v>38460</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>44752</c:v>
+                  <c:v>40380</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>46898</c:v>
+                  <c:v>40671</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>47198</c:v>
+                  <c:v>41283</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>47822</c:v>
+                  <c:v>41487</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>48100</c:v>
+                  <c:v>43548</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>50392</c:v>
+                  <c:v>43870</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>50688</c:v>
+                  <c:v>44448</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>51264</c:v>
+                  <c:v>44625</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>51326</c:v>
+                  <c:v>47041</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>53847</c:v>
+                  <c:v>47615</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1333,6 +1350,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A907-40AE-BAC3-405DCE915EF9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2076,20 +2098,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>361949</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>400051</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>128588</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2369,16 +2397,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I104"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>10444</v>
       </c>
@@ -2398,7 +2426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>10804</v>
       </c>
@@ -2424,44 +2452,50 @@
         <f>G2*E2</f>
         <v>3</v>
       </c>
-      <c r="I2">
+      <c r="J2">
+        <v>300</v>
+      </c>
+      <c r="K2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
+        <v>11819</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C56" si="0">A3-A2</f>
+        <v>1015</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E9" si="1">C3/2000</f>
+        <v>0.50749999999999995</v>
+      </c>
+      <c r="F3">
+        <v>60</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G9" si="2">F3/3.6</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H9" si="3">G3*E3</f>
+        <v>8.4583333333333339</v>
+      </c>
+      <c r="J3">
+        <v>360</v>
+      </c>
+      <c r="K3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4">
         <v>12179</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C34" si="0">A3-A2</f>
-        <v>1375</v>
-      </c>
-      <c r="E3">
-        <f>C3/2000</f>
-        <v>0.6875</v>
-      </c>
-      <c r="F3">
-        <v>61</v>
-      </c>
-      <c r="G3">
-        <f>F3/3.6</f>
-        <v>16.944444444444443</v>
-      </c>
-      <c r="H3" s="1">
-        <f>G3*E3</f>
-        <v>11.649305555555554</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>12539</v>
-      </c>
       <c r="B4">
         <v>1</v>
       </c>
@@ -2469,10 +2503,25 @@
         <f t="shared" si="0"/>
         <v>360</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>0.18</v>
+      </c>
+      <c r="F4">
+        <v>60</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>13121</v>
+        <v>12761</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2482,27 +2531,30 @@
         <v>582</v>
       </c>
       <c r="E5">
-        <f>C5/2000</f>
+        <f t="shared" si="1"/>
         <v>0.29099999999999998</v>
       </c>
       <c r="F5">
         <v>60</v>
       </c>
       <c r="G5">
-        <f>F5/3.6</f>
+        <f t="shared" si="2"/>
         <v>16.666666666666668</v>
       </c>
       <c r="H5" s="1">
-        <f>G5*E5</f>
+        <f t="shared" si="3"/>
         <v>4.8499999999999996</v>
       </c>
-      <c r="I5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>1015</v>
+      </c>
+      <c r="K5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>13421</v>
+        <v>13061</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2511,40 +2563,58 @@
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="F6">
+        <v>60</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
+      <c r="J6">
+        <v>1980</v>
+      </c>
+      <c r="K6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>15701</v>
+        <v>15041</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>2280</v>
+        <v>1980</v>
       </c>
       <c r="E7">
-        <f>C7/2000</f>
-        <v>1.1399999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.99</v>
       </c>
       <c r="F7">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7">
-        <f>F7/3.6</f>
-        <v>16.944444444444443</v>
+        <f t="shared" si="2"/>
+        <v>16.666666666666668</v>
       </c>
       <c r="H7" s="1">
-        <f>G7*E7</f>
-        <v>19.316666666666663</v>
-      </c>
-      <c r="I7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>16001</v>
+        <v>15341</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2553,10 +2623,31 @@
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="F8">
+        <v>60</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
+      <c r="J8">
+        <v>582</v>
+      </c>
+      <c r="K8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>16589</v>
+        <v>15929</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2565,10 +2656,31 @@
         <f t="shared" si="0"/>
         <v>588</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="F9">
+        <v>60</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="3"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J9">
+        <v>588</v>
+      </c>
+      <c r="K9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>16889</v>
+        <v>16229</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2577,22 +2689,28 @@
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>738</v>
+      </c>
+      <c r="K10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>19169</v>
+        <v>18209</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>19469</v>
+        <v>18509</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2602,9 +2720,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>20057</v>
+        <v>19097</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2614,9 +2732,9 @@
         <v>588</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>20357</v>
+        <v>19397</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2626,21 +2744,21 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>22637</v>
+        <v>21377</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>22937</v>
+        <v>21677</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2650,9 +2768,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>23525</v>
+        <v>22265</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2662,9 +2780,9 @@
         <v>588</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>23825</v>
+        <v>22565</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2674,21 +2792,21 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>26105</v>
+        <v>24545</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>26405</v>
+        <v>24845</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -2698,9 +2816,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>26993</v>
+        <v>25433</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2710,9 +2828,9 @@
         <v>588</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>27293</v>
+        <v>25733</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2722,21 +2840,21 @@
         <v>300</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>29573</v>
+        <v>27713</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>29873</v>
+        <v>28013</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2746,9 +2864,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>30461</v>
+        <v>28601</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2758,9 +2876,9 @@
         <v>588</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>30761</v>
+        <v>28901</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2770,21 +2888,21 @@
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>33041</v>
+        <v>30881</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>33341</v>
+        <v>31181</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -2794,9 +2912,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>33929</v>
+        <v>31769</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2806,9 +2924,9 @@
         <v>588</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>34229</v>
+        <v>32069</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -2818,21 +2936,21 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>36509</v>
+        <v>34049</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>36809</v>
+        <v>34349</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -2842,9 +2960,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>37397</v>
+        <v>34937</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -2854,9 +2972,9 @@
         <v>588</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>37697</v>
+        <v>35237</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -2866,556 +2984,674 @@
         <v>300</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>39977</v>
+        <v>37217</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>40277</v>
+        <v>37517</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>40865</v>
+        <v>38105</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>41165</v>
+        <v>38405</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>43445</v>
+        <v>40385</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>43745</v>
+        <v>40685</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>44333</v>
+        <v>41273</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>44633</v>
+        <v>41573</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>46913</v>
+        <v>43553</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>47213</v>
+        <v>43853</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>47801</v>
+        <v>44441</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46">
-        <v>48101</v>
+        <v>44741</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47">
-        <v>50381</v>
+        <v>46721</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48">
-        <v>50681</v>
+        <v>47021</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49">
-        <v>51269</v>
+        <v>47609</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50">
-        <v>51569</v>
+        <v>47909</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51">
-        <v>53849</v>
+        <v>49889</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52">
-        <v>54149</v>
+        <v>50189</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53">
-        <v>54887</v>
+        <v>50927</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>738</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54">
-        <v>55247</v>
+        <v>51287</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55">
-        <v>56622</v>
+        <v>52302</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56">
-        <v>56982</v>
+        <v>52662</v>
       </c>
       <c r="B56">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58">
-        <v>12537</v>
+        <v>10806</v>
       </c>
       <c r="B58">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59">
-        <v>13573</v>
+        <v>11809</v>
       </c>
       <c r="B59">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60">
-        <v>15697</v>
+        <v>12217</v>
       </c>
       <c r="B60">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61">
-        <v>16025</v>
+        <v>12754</v>
       </c>
       <c r="B61">
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62">
-        <v>16587</v>
+        <v>13074</v>
       </c>
       <c r="B62">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63">
-        <v>16902</v>
+        <v>15021</v>
       </c>
       <c r="B63">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64">
-        <v>19147</v>
+        <v>15339</v>
       </c>
       <c r="B64">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65">
-        <v>19474</v>
+        <v>15944</v>
       </c>
       <c r="B65">
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66">
-        <v>20085</v>
+        <v>16186</v>
       </c>
       <c r="B66">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67">
-        <v>20341</v>
+        <v>18203</v>
       </c>
       <c r="B67">
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68">
-        <v>22636</v>
+        <v>18512</v>
       </c>
       <c r="B68">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69">
-        <v>22937</v>
+        <v>19101</v>
       </c>
       <c r="B69">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70">
-        <v>23505</v>
+        <v>19393</v>
       </c>
       <c r="B70">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71">
-        <v>23856</v>
+        <v>21367</v>
       </c>
       <c r="B71">
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72">
-        <v>26105</v>
+        <v>21676</v>
       </c>
       <c r="B72">
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73">
-        <v>26404</v>
+        <v>22254</v>
       </c>
       <c r="B73">
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74">
-        <v>26956</v>
+        <v>22487</v>
       </c>
       <c r="B74">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A75">
-        <v>27241</v>
+        <v>24582</v>
       </c>
       <c r="B75">
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A76">
-        <v>29548</v>
+        <v>24913</v>
       </c>
       <c r="B76">
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A77">
-        <v>29924</v>
+        <v>25444</v>
       </c>
       <c r="B77">
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A78">
-        <v>30455</v>
+        <v>25709</v>
       </c>
       <c r="B78">
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A79">
-        <v>30770</v>
+        <v>27707</v>
       </c>
       <c r="B79">
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A80">
-        <v>33067</v>
+        <v>28015</v>
       </c>
       <c r="B80">
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A81">
-        <v>33304</v>
+        <v>28585</v>
       </c>
       <c r="B81">
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A82">
-        <v>33937</v>
+        <v>28729</v>
       </c>
       <c r="B82">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A83">
-        <v>34238</v>
+        <v>30883</v>
       </c>
       <c r="B83">
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A84">
-        <v>36521</v>
+        <v>31147</v>
       </c>
       <c r="B84">
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A85">
-        <v>36746</v>
+        <v>31784</v>
       </c>
       <c r="B85">
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A86">
-        <v>37410</v>
+        <v>32359</v>
       </c>
       <c r="B86">
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A87">
-        <v>37704</v>
+        <v>34041</v>
       </c>
       <c r="B87">
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A88">
-        <v>39965</v>
+        <v>34317</v>
       </c>
       <c r="B88">
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A89">
-        <v>40309</v>
+        <v>34933</v>
       </c>
       <c r="B89">
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A90">
-        <v>40882</v>
+        <v>35224</v>
       </c>
       <c r="B90">
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A91">
-        <v>41242</v>
+        <v>37206</v>
       </c>
       <c r="B91">
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A92">
-        <v>43437</v>
+        <v>37578</v>
       </c>
       <c r="B92">
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A93">
-        <v>43727</v>
+        <v>38106</v>
       </c>
       <c r="B93">
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A94">
-        <v>44357</v>
+        <v>38460</v>
       </c>
       <c r="B94">
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A95">
-        <v>44752</v>
+        <v>40380</v>
       </c>
       <c r="B95">
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A96">
-        <v>46898</v>
+        <v>40671</v>
       </c>
       <c r="B96">
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A97">
-        <v>47198</v>
+        <v>41283</v>
       </c>
       <c r="B97">
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A98">
-        <v>47822</v>
+        <v>41487</v>
       </c>
       <c r="B98">
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A99">
-        <v>48100</v>
+        <v>43548</v>
       </c>
       <c r="B99">
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A100">
-        <v>50392</v>
+        <v>43870</v>
       </c>
       <c r="B100">
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A101">
-        <v>50688</v>
+        <v>44448</v>
       </c>
       <c r="B101">
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A102">
-        <v>51264</v>
+        <v>44625</v>
       </c>
       <c r="B102">
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A103">
-        <v>51326</v>
+        <v>47041</v>
       </c>
       <c r="B103">
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A104">
-        <v>53847</v>
+        <v>47615</v>
       </c>
       <c r="B104">
         <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A105">
+        <v>48118</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A106">
+        <v>49860</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A107">
+        <v>50161</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A108">
+        <v>50908</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A109">
+        <v>51385</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A110">
+        <v>52322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now also does reversed cars
</commit_message>
<xml_diff>
--- a/src/a.xlsx
+++ b/src/a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\cygwin64\home\s.hein\GitHub\Trains\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{735596BE-6DD8-43A1-B4F2-38833CF488E0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{703AED12-E086-4B6C-8DF9-7E717A0F8A21}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="0" windowWidth="27870" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="0" windowWidth="27870" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <t>inter</t>
   </si>
   <si>
-    <t>inter (wrong)</t>
+    <t>count</t>
   </si>
 </sst>
 </file>
@@ -829,16 +829,16 @@
                   <c:v>50189</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>50927</c:v>
+                  <c:v>50771</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>51287</c:v>
+                  <c:v>51131</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>52302</c:v>
+                  <c:v>52146</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>52662</c:v>
+                  <c:v>52506</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1059,145 +1059,145 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="47"/>
                 <c:pt idx="0">
-                  <c:v>10806</c:v>
+                  <c:v>11812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11809</c:v>
+                  <c:v>12187</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12217</c:v>
+                  <c:v>12783</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12754</c:v>
+                  <c:v>12826</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13074</c:v>
+                  <c:v>15048</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15021</c:v>
+                  <c:v>15329</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15339</c:v>
+                  <c:v>15916</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15944</c:v>
+                  <c:v>18222</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16186</c:v>
+                  <c:v>18525</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18203</c:v>
+                  <c:v>19094</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18512</c:v>
+                  <c:v>19125</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19101</c:v>
+                  <c:v>21352</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19393</c:v>
+                  <c:v>21647</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21367</c:v>
+                  <c:v>22229</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21676</c:v>
+                  <c:v>22518</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22254</c:v>
+                  <c:v>24558</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22487</c:v>
+                  <c:v>24902</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24582</c:v>
+                  <c:v>25436</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>24913</c:v>
+                  <c:v>25546</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>25444</c:v>
+                  <c:v>27708</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25709</c:v>
+                  <c:v>28614</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>27707</c:v>
+                  <c:v>28759</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>28015</c:v>
+                  <c:v>30889</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>28585</c:v>
+                  <c:v>31222</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>28729</c:v>
+                  <c:v>31754</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>30883</c:v>
+                  <c:v>32092</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>31147</c:v>
+                  <c:v>34052</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>31784</c:v>
+                  <c:v>34363</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>32359</c:v>
+                  <c:v>34934</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>34041</c:v>
+                  <c:v>35227</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>34317</c:v>
+                  <c:v>37247</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>34933</c:v>
+                  <c:v>37512</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>35224</c:v>
+                  <c:v>38097</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>37206</c:v>
+                  <c:v>38495</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>37578</c:v>
+                  <c:v>40388</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>38106</c:v>
+                  <c:v>40695</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>38460</c:v>
+                  <c:v>41267</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>40380</c:v>
+                  <c:v>41597</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>40671</c:v>
+                  <c:v>43567</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41283</c:v>
+                  <c:v>43825</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41487</c:v>
+                  <c:v>44435</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>43548</c:v>
+                  <c:v>44780</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>43870</c:v>
+                  <c:v>46683</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>44448</c:v>
+                  <c:v>47005</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>44625</c:v>
+                  <c:v>47615</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>47041</c:v>
+                  <c:v>47839</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>47615</c:v>
+                  <c:v>49889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2398,15 +2398,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K110"/>
+  <dimension ref="A1:L110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>10444</v>
       </c>
@@ -2425,8 +2425,11 @@
       <c r="H1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>10804</v>
       </c>
@@ -2458,8 +2461,11 @@
       <c r="K2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>11819</v>
       </c>
@@ -2491,8 +2497,11 @@
       <c r="K3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>12179</v>
       </c>
@@ -2519,7 +2528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>12761</v>
       </c>
@@ -2551,8 +2560,11 @@
       <c r="K5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>13061</v>
       </c>
@@ -2584,8 +2596,11 @@
       <c r="K6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>15041</v>
       </c>
@@ -2612,7 +2627,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>15341</v>
       </c>
@@ -2644,8 +2659,11 @@
       <c r="K8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>15929</v>
       </c>
@@ -2677,8 +2695,11 @@
       <c r="K9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>16229</v>
       </c>
@@ -2689,14 +2710,8 @@
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="J10">
-        <v>738</v>
-      </c>
-      <c r="K10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>18209</v>
       </c>
@@ -2707,8 +2722,12 @@
         <f t="shared" si="0"/>
         <v>1980</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L11">
+        <f>SUM(L2:L9)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>18509</v>
       </c>
@@ -2720,7 +2739,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>19097</v>
       </c>
@@ -2732,7 +2751,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>19397</v>
       </c>
@@ -2744,7 +2763,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>21377</v>
       </c>
@@ -2756,7 +2775,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>21677</v>
       </c>
@@ -3202,19 +3221,19 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53">
-        <v>50927</v>
+        <v>50771</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
       <c r="C53">
         <f t="shared" si="0"/>
-        <v>738</v>
+        <v>582</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54">
-        <v>51287</v>
+        <v>51131</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -3226,7 +3245,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55">
-        <v>52302</v>
+        <v>52146</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -3238,7 +3257,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56">
-        <v>52662</v>
+        <v>52506</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -3250,7 +3269,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58">
-        <v>10806</v>
+        <v>11812</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -3258,7 +3277,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59">
-        <v>11809</v>
+        <v>12187</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -3266,7 +3285,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60">
-        <v>12217</v>
+        <v>12783</v>
       </c>
       <c r="B60">
         <v>2</v>
@@ -3274,7 +3293,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61">
-        <v>12754</v>
+        <v>12826</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -3282,7 +3301,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62">
-        <v>13074</v>
+        <v>15048</v>
       </c>
       <c r="B62">
         <v>2</v>
@@ -3290,7 +3309,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63">
-        <v>15021</v>
+        <v>15329</v>
       </c>
       <c r="B63">
         <v>2</v>
@@ -3298,7 +3317,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64">
-        <v>15339</v>
+        <v>15916</v>
       </c>
       <c r="B64">
         <v>2</v>
@@ -3306,7 +3325,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65">
-        <v>15944</v>
+        <v>18222</v>
       </c>
       <c r="B65">
         <v>2</v>
@@ -3314,7 +3333,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66">
-        <v>16186</v>
+        <v>18525</v>
       </c>
       <c r="B66">
         <v>2</v>
@@ -3322,7 +3341,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67">
-        <v>18203</v>
+        <v>19094</v>
       </c>
       <c r="B67">
         <v>2</v>
@@ -3330,7 +3349,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68">
-        <v>18512</v>
+        <v>19125</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -3338,7 +3357,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69">
-        <v>19101</v>
+        <v>21352</v>
       </c>
       <c r="B69">
         <v>2</v>
@@ -3346,7 +3365,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70">
-        <v>19393</v>
+        <v>21647</v>
       </c>
       <c r="B70">
         <v>2</v>
@@ -3354,7 +3373,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71">
-        <v>21367</v>
+        <v>22229</v>
       </c>
       <c r="B71">
         <v>2</v>
@@ -3362,7 +3381,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72">
-        <v>21676</v>
+        <v>22518</v>
       </c>
       <c r="B72">
         <v>2</v>
@@ -3370,7 +3389,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73">
-        <v>22254</v>
+        <v>24558</v>
       </c>
       <c r="B73">
         <v>2</v>
@@ -3378,7 +3397,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74">
-        <v>22487</v>
+        <v>24902</v>
       </c>
       <c r="B74">
         <v>2</v>
@@ -3386,7 +3405,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A75">
-        <v>24582</v>
+        <v>25436</v>
       </c>
       <c r="B75">
         <v>2</v>
@@ -3394,7 +3413,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A76">
-        <v>24913</v>
+        <v>25546</v>
       </c>
       <c r="B76">
         <v>2</v>
@@ -3402,7 +3421,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A77">
-        <v>25444</v>
+        <v>27708</v>
       </c>
       <c r="B77">
         <v>2</v>
@@ -3410,7 +3429,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A78">
-        <v>25709</v>
+        <v>28614</v>
       </c>
       <c r="B78">
         <v>2</v>
@@ -3418,7 +3437,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A79">
-        <v>27707</v>
+        <v>28759</v>
       </c>
       <c r="B79">
         <v>2</v>
@@ -3426,7 +3445,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A80">
-        <v>28015</v>
+        <v>30889</v>
       </c>
       <c r="B80">
         <v>2</v>
@@ -3434,7 +3453,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A81">
-        <v>28585</v>
+        <v>31222</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -3442,7 +3461,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A82">
-        <v>28729</v>
+        <v>31754</v>
       </c>
       <c r="B82">
         <v>2</v>
@@ -3450,7 +3469,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A83">
-        <v>30883</v>
+        <v>32092</v>
       </c>
       <c r="B83">
         <v>2</v>
@@ -3458,7 +3477,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A84">
-        <v>31147</v>
+        <v>34052</v>
       </c>
       <c r="B84">
         <v>2</v>
@@ -3466,7 +3485,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A85">
-        <v>31784</v>
+        <v>34363</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -3474,7 +3493,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A86">
-        <v>32359</v>
+        <v>34934</v>
       </c>
       <c r="B86">
         <v>2</v>
@@ -3482,7 +3501,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A87">
-        <v>34041</v>
+        <v>35227</v>
       </c>
       <c r="B87">
         <v>2</v>
@@ -3490,7 +3509,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A88">
-        <v>34317</v>
+        <v>37247</v>
       </c>
       <c r="B88">
         <v>2</v>
@@ -3498,7 +3517,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A89">
-        <v>34933</v>
+        <v>37512</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -3506,7 +3525,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A90">
-        <v>35224</v>
+        <v>38097</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -3514,7 +3533,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A91">
-        <v>37206</v>
+        <v>38495</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -3522,7 +3541,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A92">
-        <v>37578</v>
+        <v>40388</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -3530,7 +3549,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A93">
-        <v>38106</v>
+        <v>40695</v>
       </c>
       <c r="B93">
         <v>2</v>
@@ -3538,7 +3557,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A94">
-        <v>38460</v>
+        <v>41267</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -3546,7 +3565,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A95">
-        <v>40380</v>
+        <v>41597</v>
       </c>
       <c r="B95">
         <v>2</v>
@@ -3554,7 +3573,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A96">
-        <v>40671</v>
+        <v>43567</v>
       </c>
       <c r="B96">
         <v>2</v>
@@ -3562,7 +3581,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A97">
-        <v>41283</v>
+        <v>43825</v>
       </c>
       <c r="B97">
         <v>2</v>
@@ -3570,7 +3589,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A98">
-        <v>41487</v>
+        <v>44435</v>
       </c>
       <c r="B98">
         <v>2</v>
@@ -3578,7 +3597,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A99">
-        <v>43548</v>
+        <v>44780</v>
       </c>
       <c r="B99">
         <v>2</v>
@@ -3586,7 +3605,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A100">
-        <v>43870</v>
+        <v>46683</v>
       </c>
       <c r="B100">
         <v>2</v>
@@ -3594,7 +3613,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A101">
-        <v>44448</v>
+        <v>47005</v>
       </c>
       <c r="B101">
         <v>2</v>
@@ -3602,7 +3621,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A102">
-        <v>44625</v>
+        <v>47615</v>
       </c>
       <c r="B102">
         <v>2</v>
@@ -3610,7 +3629,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A103">
-        <v>47041</v>
+        <v>47839</v>
       </c>
       <c r="B103">
         <v>2</v>
@@ -3618,7 +3637,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A104">
-        <v>47615</v>
+        <v>49889</v>
       </c>
       <c r="B104">
         <v>2</v>
@@ -3626,22 +3645,22 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A105">
-        <v>48118</v>
+        <v>50250</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A106">
-        <v>49860</v>
+        <v>50794</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A107">
-        <v>50161</v>
+        <v>51162</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A108">
-        <v>50908</v>
+        <v>52167</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Fixed the negative-interval problem
</commit_message>
<xml_diff>
--- a/src/a.xlsx
+++ b/src/a.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\cygwin64\home\s.hein\GitHub\Trains\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cygwin64\home\heins\GitHub\Trains\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{703AED12-E086-4B6C-8DF9-7E717A0F8A21}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="0" windowWidth="27870" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="0" windowWidth="27870" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="1" r:id="rId1"/>
@@ -49,7 +48,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -592,7 +591,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -606,6 +605,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1021,7 +1021,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A907-40AE-BAC3-405DCE915EF9}"/>
             </c:ext>
@@ -1350,7 +1350,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-A907-40AE-BAC3-405DCE915EF9}"/>
             </c:ext>
@@ -1364,11 +1364,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="523163000"/>
-        <c:axId val="523152808"/>
+        <c:axId val="524069064"/>
+        <c:axId val="524065144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="523163000"/>
+        <c:axId val="524069064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1425,14 +1425,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="523152808"/>
+        <c:crossAx val="524065144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4000"/>
         <c:minorUnit val="1000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="523152808"/>
+        <c:axId val="524065144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1489,7 +1489,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="523163000"/>
+        <c:crossAx val="524069064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2114,7 +2114,7 @@
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2397,16 +2397,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>10444</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10804</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11819</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12179</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>12761</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>13061</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>15041</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>15341</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>15929</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>16229</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>18209</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>18509</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>19097</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>19397</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>21377</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>21677</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>22265</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>22565</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>24545</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>24845</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>25433</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>25733</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>27713</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>28013</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>28601</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>28901</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>30881</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>31181</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>31769</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>32069</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>34049</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>34349</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>34937</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>35237</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>37217</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>37517</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>38105</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38405</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>40385</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40685</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>41273</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41573</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>43553</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43853</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44441</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44741</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46721</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47021</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47609</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>47909</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49889</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50189</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50771</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>51131</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>52146</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>52506</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>11812</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>12187</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>12783</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>12826</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>15048</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>15329</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>15916</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>18222</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>18525</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>19094</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>19125</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>21352</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>21647</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>22229</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>22518</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>24558</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>24902</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>25436</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>25546</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>27708</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>28614</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>28759</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>30889</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>31222</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>31754</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>32092</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>34052</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>34363</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>34934</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>35227</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>37247</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>37512</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>38097</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>38495</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>40388</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>40695</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>41267</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>41597</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>43567</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>43825</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>44435</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>44780</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>46683</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>47005</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>47615</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>47839</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>49889</v>
       </c>
@@ -3643,32 +3643,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>50250</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>50794</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>51162</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>52167</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>51385</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>52322</v>
       </c>

</xml_diff>